<commit_message>
Killed the bug of IdMaster
</commit_message>
<xml_diff>
--- a/SpecForTablesxlsx.xlsx
+++ b/SpecForTablesxlsx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="10620" windowHeight="5400" tabRatio="742" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="10620" windowHeight="5400" tabRatio="742" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ID" sheetId="1" r:id="rId1"/>
@@ -1372,7 +1372,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2286,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3014,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3378,7 +3378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>